<commit_message>
Fixed time calculation and pie charts
</commit_message>
<xml_diff>
--- a/docs/01-basics/pie-chart-overview.xlsx
+++ b/docs/01-basics/pie-chart-overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Documents/developer/github_isaqb/advanced-template/docs/01-basics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/dev/isaqb/curriculum-flex/docs/01-basics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B0021D-F328-FD4D-84C2-7CEE7CC41D66}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286E8B38-CD4D-294C-9985-7EC7B37C4704}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1900" windowWidth="24560" windowHeight="17660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4240" yWindow="460" windowWidth="24560" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DE-Grafik" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Vortrag</t>
   </si>
@@ -47,24 +47,6 @@
     <t>Gesamt</t>
   </si>
   <si>
-    <t>Thema mit Einleitung</t>
-  </si>
-  <si>
-    <t>Thema über xz</t>
-  </si>
-  <si>
-    <t>Thema mit viel Theorie</t>
-  </si>
-  <si>
-    <t>Thema mit xy und Beispiel</t>
-  </si>
-  <si>
-    <t>Thema mit abc und d</t>
-  </si>
-  <si>
-    <t>Thema mit Abschlussbeispiel</t>
-  </si>
-  <si>
     <t>Introduction</t>
   </si>
   <si>
@@ -81,6 +63,27 @@
   </si>
   <si>
     <t>final example</t>
+  </si>
+  <si>
+    <t>Motivation</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>Case Study</t>
+  </si>
+  <si>
+    <t>Modularization</t>
+  </si>
+  <si>
+    <t>Operations, Monitoring, and Failure Analysis</t>
+  </si>
+  <si>
+    <t>Installation and Rollout</t>
+  </si>
+  <si>
+    <t>Forecast</t>
   </si>
 </sst>
 </file>
@@ -377,22 +380,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Thema mit Einleitung</c:v>
+                  <c:v>Motivation</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Thema über xz</c:v>
+                  <c:v>Modularization</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Thema mit viel Theorie</c:v>
+                  <c:v>Integration</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Thema mit xy und Beispiel</c:v>
+                  <c:v>Operations, Monitoring, and Failure Analysis</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Thema mit abc und d</c:v>
+                  <c:v>Installation and Rollout</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Thema mit Abschlussbeispiel</c:v>
+                  <c:v>Case Study</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -404,22 +407,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>180</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>120</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>180</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>210</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>120</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -801,13 +804,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1201,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C6"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1215,56 +1218,64 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B1">
-        <v>180</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>150</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B4">
-        <v>180</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B5">
-        <v>210</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <f>SUM(B1:B6)</f>
-        <v>960</v>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f>SUM(B1:B7)</f>
+        <v>1080</v>
       </c>
     </row>
   </sheetData>
@@ -1290,7 +1301,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B1">
         <v>180</v>
@@ -1298,7 +1309,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>150</v>
@@ -1306,7 +1317,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>120</v>
@@ -1314,7 +1325,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>180</v>
@@ -1322,7 +1333,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>210</v>
@@ -1330,7 +1341,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>120</v>

</xml_diff>

<commit_message>
Merged changes from master branch
</commit_message>
<xml_diff>
--- a/docs/01-basics/pie-chart-overview.xlsx
+++ b/docs/01-basics/pie-chart-overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Documents/developer/github_isaqb/advanced-template/docs/01-basics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/dev/isaqb/curriculum-flex/docs/01-basics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B0021D-F328-FD4D-84C2-7CEE7CC41D66}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB852A38-F12F-114D-A1F6-3DF74861E1D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1900" windowWidth="24560" windowHeight="17660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4240" yWindow="460" windowWidth="24560" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DE-Grafik" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Vortrag</t>
   </si>
@@ -47,40 +47,34 @@
     <t>Gesamt</t>
   </si>
   <si>
-    <t>Thema mit Einleitung</t>
+    <t>Motivation</t>
   </si>
   <si>
-    <t>Thema über xz</t>
+    <t>Integration</t>
   </si>
   <si>
-    <t>Thema mit viel Theorie</t>
+    <t>Case Study</t>
   </si>
   <si>
-    <t>Thema mit xy und Beispiel</t>
+    <t>Modularization</t>
   </si>
   <si>
-    <t>Thema mit abc und d</t>
+    <t>Operations, Monitoring, and Failure Analysis</t>
   </si>
   <si>
-    <t>Thema mit Abschlussbeispiel</t>
+    <t>Installation and Rollout</t>
   </si>
   <si>
-    <t>Introduction</t>
+    <t>Forecast</t>
   </si>
   <si>
-    <t>xz</t>
+    <t>Modularisierung</t>
   </si>
   <si>
-    <t>Lots of theory</t>
+    <t>Betrieb, Überwachung und Fehleranalyse</t>
   </si>
   <si>
-    <t>xy and example</t>
-  </si>
-  <si>
-    <t>abc and d</t>
-  </si>
-  <si>
-    <t>final example</t>
+    <t>Ausblick</t>
   </si>
 </sst>
 </file>
@@ -377,22 +371,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Thema mit Einleitung</c:v>
+                  <c:v>Motivation</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Thema über xz</c:v>
+                  <c:v>Modularisierung</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Thema mit viel Theorie</c:v>
+                  <c:v>Integration</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Thema mit xy und Beispiel</c:v>
+                  <c:v>Betrieb, Überwachung und Fehleranalyse</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Thema mit abc und d</c:v>
+                  <c:v>Installation and Rollout</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Thema mit Abschlussbeispiel</c:v>
+                  <c:v>Case Study</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -404,22 +398,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>180</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>120</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>180</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>210</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>120</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -703,22 +697,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Introduction</c:v>
+                  <c:v>Motivation</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>xz</c:v>
+                  <c:v>Modularization</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Lots of theory</c:v>
+                  <c:v>Integration</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>xy and example</c:v>
+                  <c:v>Operations, Monitoring, and Failure Analysis</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>abc and d</c:v>
+                  <c:v>Installation and Rollout</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>final example</c:v>
+                  <c:v>Case Study</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -730,22 +724,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>180</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>120</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>180</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>210</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>120</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -801,13 +795,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1201,10 +1195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1218,53 +1212,61 @@
         <v>3</v>
       </c>
       <c r="B1">
-        <v>180</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>150</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>180</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>210</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <f>SUM(B1:B6)</f>
-        <v>960</v>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f>SUM(B1:B7)</f>
+        <v>1080</v>
       </c>
     </row>
   </sheetData>
@@ -1276,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1290,56 +1292,64 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B1">
-        <v>180</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>150</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>180</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>210</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <f>SUM(B1:B6)</f>
-        <v>960</v>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f>SUM(B1:B7)</f>
+        <v>1080</v>
       </c>
     </row>
   </sheetData>

</xml_diff>